<commit_message>
backup 2 juni 2025
</commit_message>
<xml_diff>
--- a/reverse/data_gempa.xlsx
+++ b/reverse/data_gempa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KULIAH\Skripsi\reverse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C967F6-658E-47FC-A290-97DFC2401A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9813BDF3-23F9-435D-B900-FA7AC5E73355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4F113E1E-B4B7-40FC-A4E8-D78020222ADA}"/>
   </bookViews>
@@ -8901,7 +8901,7 @@
   <dimension ref="A1:G2856"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -58284,6 +58284,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>